<commit_message>
EURent - next steps (not yet complete, but better than last one)
</commit_message>
<xml_diff>
--- a/Examples/EURent/EURent-Demo.xlsx
+++ b/Examples/EURent/EURent-Demo.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7896"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7896" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
-    <sheet name="Blad3" sheetId="3" r:id="rId3"/>
+    <sheet name="Statical information" sheetId="1" r:id="rId1"/>
+    <sheet name="Rentals" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="95">
   <si>
     <t>maxRentalDuration</t>
   </si>
@@ -196,13 +195,118 @@
   </si>
   <si>
     <t>LicensePlate</t>
+  </si>
+  <si>
+    <t>1-AMS-10</t>
+  </si>
+  <si>
+    <t>[Rentals]</t>
+  </si>
+  <si>
+    <t>RentalCase</t>
+  </si>
+  <si>
+    <t>rcStartDate</t>
+  </si>
+  <si>
+    <t>rcEndDate</t>
+  </si>
+  <si>
+    <t>rcCarType</t>
+  </si>
+  <si>
+    <t>rcPickupBranch</t>
+  </si>
+  <si>
+    <t>rcDropOffBranch</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>rcRenter</t>
+  </si>
+  <si>
+    <t>rcDriver</t>
+  </si>
+  <si>
+    <t>rcDrivingLicense</t>
+  </si>
+  <si>
+    <t>DrivingLicense</t>
+  </si>
+  <si>
+    <t>PersonRef</t>
+  </si>
+  <si>
+    <t>rcAssignedCar</t>
+  </si>
+  <si>
+    <t>[Transactions]</t>
+  </si>
+  <si>
+    <t>rcIsClean</t>
+  </si>
+  <si>
+    <t>rentalHasBeenRequested</t>
+  </si>
+  <si>
+    <t>rentalHasBeenPromised</t>
+  </si>
+  <si>
+    <t>rcKeysHandedOver</t>
+  </si>
+  <si>
+    <t>rentalCarHasBeenPickedUp</t>
+  </si>
+  <si>
+    <t>rentalHasBeenStarted</t>
+  </si>
+  <si>
+    <t>rc_test_1</t>
+  </si>
+  <si>
+    <t>Dick River</t>
+  </si>
+  <si>
+    <t>DL-1235-1263</t>
+  </si>
+  <si>
+    <t>&lt;- car is in a rental, see sheet 'Rentals'</t>
+  </si>
+  <si>
+    <t>rcAuthorAcc</t>
+  </si>
+  <si>
+    <t>Acc_dick</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>rc_test_2</t>
+  </si>
+  <si>
+    <t>rc_test_3</t>
+  </si>
+  <si>
+    <t>Richard Enter</t>
+  </si>
+  <si>
+    <t>Acc_richard</t>
+  </si>
+  <si>
+    <t>rc_test_4</t>
+  </si>
+  <si>
+    <t>DL-8888-9999</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,8 +329,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +348,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -263,11 +380,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -280,8 +398,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -582,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1099,10 +1236,10 @@
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF($B30="","",$B30)</f>
-        <v>1-AMS-11</v>
+        <v>1-AMS-10</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>29</v>
@@ -1110,32 +1247,33 @@
       <c r="D30" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
-        <f t="shared" ref="A31:A38" si="4">IF($B31="","",$B31)</f>
-        <v>1-AMS-12</v>
+        <f>IF($B31="","",$B31)</f>
+        <v>1-AMS-11</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>16</v>
+      <c r="E31" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
-        <f t="shared" si="4"/>
-        <v>1-AMS-13</v>
+        <f t="shared" ref="A32:A39" si="4">IF($B32="","",$B32)</f>
+        <v>1-AMS-12</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>16</v>
@@ -1144,91 +1282,106 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f t="shared" si="4"/>
-        <v>2-DHG-14</v>
+        <v>1-AMS-13</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f t="shared" si="4"/>
-        <v>2-DHG-15</v>
+        <v>2-DHG-14</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f t="shared" si="4"/>
-        <v>2-DHG-16</v>
+        <v>2-DHG-15</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f t="shared" si="4"/>
-        <v>3-RTD-17</v>
+        <v>2-DHG-16</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f t="shared" si="4"/>
-        <v>3-RTD-18</v>
+        <v>3-RTD-17</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f t="shared" si="4"/>
+        <v>3-RTD-18</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
+        <f t="shared" si="4"/>
         <v>3-RTD-19</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1240,24 +1393,470 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15:L15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="10">
+        <f ca="1">TODAY()</f>
+        <v>42717</v>
+      </c>
+      <c r="G3" s="10">
+        <f ca="1">TODAY()+9</f>
+        <v>42726</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="10">
+        <f ca="1">TODAY()</f>
+        <v>42717</v>
+      </c>
+      <c r="G4" s="10">
+        <f ca="1">TODAY()+9</f>
+        <v>42726</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="10">
+        <f ca="1">TODAY()</f>
+        <v>42717</v>
+      </c>
+      <c r="G5" s="10">
+        <f ca="1">TODAY()+9</f>
+        <v>42726</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="10">
+        <f ca="1">TODAY()</f>
+        <v>42717</v>
+      </c>
+      <c r="G6" s="10">
+        <f ca="1">TODAY()+9</f>
+        <v>42726</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="str">
+        <f>IF($A3="","",$A3)</f>
+        <v>rc_test_1</v>
+      </c>
+      <c r="B12" s="9" t="str">
+        <f>$A12</f>
+        <v>rc_test_1</v>
+      </c>
+      <c r="D12" s="9" t="str">
+        <f t="shared" ref="D12:D18" si="0">$A12</f>
+        <v>rc_test_1</v>
+      </c>
+      <c r="F12" s="9" t="str">
+        <f t="shared" ref="F12:F18" si="1">$A12</f>
+        <v>rc_test_1</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="str">
+        <f t="shared" ref="A13:A18" si="2">IF($A4="","",$A4)</f>
+        <v>rc_test_2</v>
+      </c>
+      <c r="B13" s="9" t="str">
+        <f t="shared" ref="B13:B18" si="3">$A13</f>
+        <v>rc_test_2</v>
+      </c>
+      <c r="D13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>rc_test_2</v>
+      </c>
+      <c r="F13" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>rc_test_2</v>
+      </c>
+      <c r="H13" s="9" t="str">
+        <f t="shared" ref="H12:L18" si="4">$A13</f>
+        <v>rc_test_2</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>rc_test_3</v>
+      </c>
+      <c r="B14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>rc_test_3</v>
+      </c>
+      <c r="D14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>rc_test_3</v>
+      </c>
+      <c r="F14" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>rc_test_3</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>rc_test_4</v>
+      </c>
+      <c r="B15" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>rc_test_4</v>
+      </c>
+      <c r="D15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>rc_test_4</v>
+      </c>
+      <c r="F15" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>rc_test_4</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="B16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="D16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F16" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H16" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="J16" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L16" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="B17" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="D17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F17" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="J17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="B18" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="D18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F18" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H18" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="J18" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L18" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EURent - apart from some (ticketed) bugs in the tools, this should work. The README file needs some work though.
</commit_message>
<xml_diff>
--- a/Examples/EURent/EURent-Demo.xlsx
+++ b/Examples/EURent/EURent-Demo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7896" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Statical information" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="96">
   <si>
     <t>maxRentalDuration</t>
   </si>
@@ -272,9 +272,6 @@
     <t>DL-1235-1263</t>
   </si>
   <si>
-    <t>&lt;- car is in a rental, see sheet 'Rentals'</t>
-  </si>
-  <si>
     <t>rcAuthorAcc</t>
   </si>
   <si>
@@ -300,6 +297,12 @@
   </si>
   <si>
     <t>DL-8888-9999</t>
+  </si>
+  <si>
+    <t>rc_test_5</t>
+  </si>
+  <si>
+    <t>&lt;- car is in a STARTED rental (meaning that the keys have been handed over etc.), see sheet 'Rentals'</t>
   </si>
 </sst>
 </file>
@@ -721,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -1244,10 +1247,9 @@
       <c r="C30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="8"/>
+      <c r="E30" s="8" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
@@ -1260,9 +1262,10 @@
       <c r="C31" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="D31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
@@ -1395,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:L15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1420,7 +1423,7 @@
         <v>61</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>69</v>
@@ -1455,7 +1458,7 @@
         <v>62</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>73</v>
@@ -1490,7 +1493,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>83</v>
@@ -1503,15 +1506,18 @@
       </c>
       <c r="F3" s="10">
         <f ca="1">TODAY()</f>
-        <v>42717</v>
+        <v>42718</v>
       </c>
       <c r="G3" s="10">
         <f ca="1">TODAY()+9</f>
-        <v>42726</v>
+        <v>42727</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="I3" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="J3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1521,10 +1527,10 @@
     </row>
     <row r="4" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>83</v>
@@ -1537,11 +1543,11 @@
       </c>
       <c r="F4" s="10">
         <f ca="1">TODAY()</f>
-        <v>42717</v>
+        <v>42718</v>
       </c>
       <c r="G4" s="10">
         <f ca="1">TODAY()+9</f>
-        <v>42726</v>
+        <v>42727</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>29</v>
@@ -1558,13 +1564,13 @@
     </row>
     <row r="5" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>83</v>
@@ -1574,14 +1580,17 @@
       </c>
       <c r="F5" s="10">
         <f ca="1">TODAY()</f>
-        <v>42717</v>
+        <v>42718</v>
       </c>
       <c r="G5" s="10">
         <f ca="1">TODAY()+9</f>
-        <v>42726</v>
+        <v>42727</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>16</v>
@@ -1592,27 +1601,27 @@
     </row>
     <row r="6" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="F6" s="10">
         <f ca="1">TODAY()</f>
-        <v>42717</v>
+        <v>42718</v>
       </c>
       <c r="G6" s="10">
         <f ca="1">TODAY()+9</f>
-        <v>42726</v>
+        <v>42727</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>31</v>
@@ -1625,7 +1634,38 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="10">
+        <f ca="1">TODAY()</f>
+        <v>42718</v>
+      </c>
+      <c r="G7" s="10">
+        <f ca="1">TODAY()+9</f>
+        <v>42727</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
@@ -1696,17 +1736,26 @@
         <f t="shared" ref="F12:F18" si="1">$A12</f>
         <v>rc_test_1</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="H12" s="9" t="str">
+        <f t="shared" ref="H12:H18" si="2">$A12</f>
+        <v>rc_test_1</v>
+      </c>
+      <c r="J12" s="9" t="str">
+        <f t="shared" ref="J12" si="3">IF($H12="","",$H12)</f>
+        <v>rc_test_1</v>
+      </c>
+      <c r="L12" s="9" t="str">
+        <f>IF($J12="","",$J12)</f>
+        <v>rc_test_1</v>
+      </c>
     </row>
     <row r="13" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="str">
-        <f t="shared" ref="A13:A18" si="2">IF($A4="","",$A4)</f>
+        <f t="shared" ref="A13:A18" si="4">IF($A4="","",$A4)</f>
         <v>rc_test_2</v>
       </c>
       <c r="B13" s="9" t="str">
-        <f t="shared" ref="B13:B18" si="3">$A13</f>
+        <f t="shared" ref="B13:B18" si="5">$A13</f>
         <v>rc_test_2</v>
       </c>
       <c r="D13" s="9" t="str">
@@ -1717,20 +1766,23 @@
         <f t="shared" si="1"/>
         <v>rc_test_2</v>
       </c>
-      <c r="H13" s="9" t="str">
-        <f t="shared" ref="H12:L18" si="4">$A13</f>
-        <v>rc_test_2</v>
-      </c>
-      <c r="J13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="J13" s="9" t="str">
+        <f>IF($H13="","",$H13)</f>
+        <v/>
+      </c>
+      <c r="L13" s="9" t="str">
+        <f t="shared" ref="L13:L18" si="6">IF($J13="","",$J13)</f>
+        <v/>
+      </c>
     </row>
     <row r="14" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>rc_test_3</v>
       </c>
       <c r="B14" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>rc_test_3</v>
       </c>
       <c r="D14" s="9" t="str">
@@ -1742,16 +1794,22 @@
         <v>rc_test_3</v>
       </c>
       <c r="H14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="L14" s="9"/>
+      <c r="J14" s="9" t="str">
+        <f t="shared" ref="J14:J18" si="7">IF($H14="","",$H14)</f>
+        <v/>
+      </c>
+      <c r="L14" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>rc_test_4</v>
       </c>
       <c r="B15" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>rc_test_4</v>
       </c>
       <c r="D15" s="9" t="str">
@@ -1763,46 +1821,49 @@
         <v>rc_test_4</v>
       </c>
       <c r="H15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="L15" s="9"/>
+      <c r="J15" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L15" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>rc_test_5</v>
       </c>
       <c r="B16" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" si="5"/>
+        <v>rc_test_5</v>
       </c>
       <c r="D16" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>rc_test_5</v>
       </c>
       <c r="F16" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H16" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+        <v>rc_test_5</v>
+      </c>
+      <c r="H16" s="9"/>
       <c r="J16" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L16" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B17" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D17" s="9" t="str">
@@ -1814,25 +1875,25 @@
         <v/>
       </c>
       <c r="H17" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J17" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L17" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B18" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D18" s="9" t="str">
@@ -1844,15 +1905,15 @@
         <v/>
       </c>
       <c r="H18" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J18" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L18" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>

</xml_diff>